<commit_message>
Save outputs to subfolder data/results/<model_name>/<val> or <test>
</commit_message>
<xml_diff>
--- a/paper/DepthNet.xlsx
+++ b/paper/DepthNet.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Documents/Stanford/ares/spad_single/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F5508C-3FBB-2444-B297-C665B61EC50B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D75D7484-F9EF-AE4B-8FE0-0DAECD5E2B28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{777694D5-0BD5-8249-BEEC-1B33D94A54A3}"/>
+    <workbookView xWindow="9600" yWindow="460" windowWidth="19200" windowHeight="17540" xr2:uid="{777694D5-0BD5-8249-BEEC-1B33D94A54A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
-    <sheet name="Papers" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>DORN</t>
   </si>
@@ -68,21 +67,41 @@
     <t>mse</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Eigen et. al.</t>
   </si>
   <si>
-    <t>FCRN</t>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Laina et. al.</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>DORN + Histogram Rescaling (No noise, no albedo, no falloff)</t>
+  </si>
+  <si>
+    <t>From Papers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -110,8 +129,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFB707D8-7A70-7644-B29D-168617A77793}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -511,10 +531,10 @@
       <c r="C3">
         <v>0.96944912802694005</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>0.99173865280806295</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>0.31519769788998397</v>
       </c>
       <c r="F3">
@@ -523,7 +543,7 @@
       <c r="G3">
         <v>0.132700438813697</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="1">
         <v>8.7233799126843703E-2</v>
       </c>
       <c r="I3">
@@ -565,69 +585,137 @@
         <v>0.19988755560271901</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9384A44E-53E2-5446-A5F5-52F959CAFD26}">
-  <dimension ref="A1:J4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="39" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.89902345485840895</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.96994871391908999</v>
+      </c>
+      <c r="D5">
+        <v>0.98954798995482196</v>
+      </c>
+      <c r="E5">
+        <v>0.3224211819335</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.48643683646165198</v>
+      </c>
+      <c r="G5" s="1">
+        <v>9.4712523271281601E-2</v>
+      </c>
+      <c r="H5">
+        <v>8.8471443711215E-2</v>
+      </c>
+      <c r="I5" s="1">
+        <v>4.1298458006384701E-2</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.14785928237148899</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="C10">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="D10">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="E10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="F10">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="G10">
+        <v>0.115</v>
+      </c>
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="J10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>15</v>
+      </c>
+      <c r="B11">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="C11">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="D11">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="G11">
+        <v>0.127</v>
+      </c>
+      <c r="H11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11">
+        <v>5.5E-2</v>
+      </c>
+      <c r="J11" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SGD method converges under no-albedo, no-falloff, no-noise conditions.
</commit_message>
<xml_diff>
--- a/paper/DepthNet.xlsx
+++ b/paper/DepthNet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Documents/Stanford/ares/spad_single/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0CD4DB-2CFD-4F41-8D66-6A5264776626}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A89A5C-D4AF-0F48-ADC3-F144B8EAB515}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="460" windowWidth="19200" windowHeight="17540" xr2:uid="{777694D5-0BD5-8249-BEEC-1B33D94A54A3}"/>
+    <workbookView xWindow="24800" yWindow="5860" windowWidth="19200" windowHeight="17540" xr2:uid="{777694D5-0BD5-8249-BEEC-1B33D94A54A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="25">
   <si>
     <t>DORN</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>NYU Depth v2 Small Test Set (1000 entries)</t>
+  </si>
+  <si>
+    <t>DORN_nohints</t>
   </si>
 </sst>
 </file>
@@ -460,7 +463,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -825,6 +828,38 @@
         <v>9.6247356015322097E-2</v>
       </c>
     </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>0.97945953669757002</v>
+      </c>
+      <c r="C21">
+        <v>0.994678041453117</v>
+      </c>
+      <c r="D21">
+        <v>0.99806731906079904</v>
+      </c>
+      <c r="E21">
+        <v>0.118581589964839</v>
+      </c>
+      <c r="F21">
+        <v>0.30914099379332699</v>
+      </c>
+      <c r="G21">
+        <v>8.4022855021325601E-2</v>
+      </c>
+      <c r="H21">
+        <v>3.1475905720026003E-2</v>
+      </c>
+      <c r="I21">
+        <v>3.8626020417079E-2</v>
+      </c>
+      <c r="J21">
+        <v>0.105912321823124</v>
+      </c>
+    </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>23</v>
@@ -923,7 +958,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B31">
         <v>0.81476784850522999</v>

</xml_diff>

<commit_message>
Downloaded and processed nyuv2 labeled dataset.
</commit_message>
<xml_diff>
--- a/paper/DepthNet.xlsx
+++ b/paper/DepthNet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Documents/Stanford/ares/spad_single/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68494B47-66ED-BD45-9188-7C5E7F430BA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F2A812-E85A-1942-9757-78B11BD38EDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6840" yWindow="3300" windowWidth="28800" windowHeight="17540" xr2:uid="{777694D5-0BD5-8249-BEEC-1B33D94A54A3}"/>
+    <workbookView xWindow="15780" yWindow="2100" windowWidth="28800" windowHeight="17540" xr2:uid="{777694D5-0BD5-8249-BEEC-1B33D94A54A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="43">
   <si>
     <t>DORN</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>DORN + Median Rescaling</t>
+  </si>
+  <si>
+    <t>Hu, Ozay et. al. (2018) Revisiting Single Image Depth Estimation</t>
   </si>
 </sst>
 </file>
@@ -523,7 +526,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -982,6 +985,29 @@
       </c>
       <c r="I15" s="4">
         <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0.115</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0.05</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Ran DORN and DenseDepth on nohints dataset.
</commit_message>
<xml_diff>
--- a/paper/DepthNet.xlsx
+++ b/paper/DepthNet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Documents/Stanford/ares/spad_single/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F2A812-E85A-1942-9757-78B11BD38EDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A26B8D-0881-B545-9A78-7DABC13F4799}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15780" yWindow="2100" windowWidth="28800" windowHeight="17540" xr2:uid="{777694D5-0BD5-8249-BEEC-1B33D94A54A3}"/>
+    <workbookView xWindow="-21280" yWindow="3320" windowWidth="28800" windowHeight="17540" xr2:uid="{777694D5-0BD5-8249-BEEC-1B33D94A54A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="48">
   <si>
     <t>DORN</t>
   </si>
@@ -155,6 +155,21 @@
   </si>
   <si>
     <t>Hu, Ozay et. al. (2018) Revisiting Single Image Depth Estimation</t>
+  </si>
+  <si>
+    <t>NYU Depth v2 Labled Test Set (654 Entries)</t>
+  </si>
+  <si>
+    <t>rel_abs_dif</t>
+  </si>
+  <si>
+    <t>DenseDepth_nohints</t>
+  </si>
+  <si>
+    <t>Uses rawdepth for evaluation (masks off invalid depth pixels), unlike what Wonka et.al. do in their paper.</t>
+  </si>
+  <si>
+    <t>Pytorch version. Will run caffe version soon.</t>
   </si>
 </sst>
 </file>
@@ -523,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFB707D8-7A70-7644-B29D-168617A77793}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1242,7 +1257,7 @@
         <v>0.17088902548313301</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -1272,6 +1287,110 @@
       </c>
       <c r="J33" s="2">
         <v>0.186160584261236</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" s="2">
+        <v>0.83929108669991404</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.95858464605035199</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.98564354107743601</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0.26140680609123301</v>
+      </c>
+      <c r="F37" s="2">
+        <f>SQRT(E37)</f>
+        <v>0.51127957722877315</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0.12950759483657001</v>
+      </c>
+      <c r="H37" s="2">
+        <v>8.7568223680133297E-2</v>
+      </c>
+      <c r="I37" s="2">
+        <v>5.8503517225143298E-2</v>
+      </c>
+      <c r="J37" s="2">
+        <v>0.17285743104927601</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0.85618639232578697</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.97836328187102095</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.99565340722963402</v>
+      </c>
+      <c r="E38" s="2">
+        <v>0.21353111323962001</v>
+      </c>
+      <c r="F38" s="2">
+        <f>SQRT(E38)</f>
+        <v>0.4620942687803215</v>
+      </c>
+      <c r="G38" s="2">
+        <v>0.11950074903631699</v>
+      </c>
+      <c r="H38" s="2">
+        <v>6.8724721778946202E-2</v>
+      </c>
+      <c r="I38" s="2">
+        <v>5.1383407905070101E-2</v>
+      </c>
+      <c r="J38" s="2">
+        <v>0.151374158361015</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DenseDepth matches github evaluation script.
</commit_message>
<xml_diff>
--- a/paper/DepthNet.xlsx
+++ b/paper/DepthNet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Documents/Stanford/ares/spad_single/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A26B8D-0881-B545-9A78-7DABC13F4799}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A5E402-A504-B249-B436-9C705D1309F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21280" yWindow="3320" windowWidth="28800" windowHeight="17540" xr2:uid="{777694D5-0BD5-8249-BEEC-1B33D94A54A3}"/>
+    <workbookView xWindow="5420" yWindow="1480" windowWidth="28800" windowHeight="17540" xr2:uid="{777694D5-0BD5-8249-BEEC-1B33D94A54A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="51">
   <si>
     <t>DORN</t>
   </si>
@@ -163,13 +163,22 @@
     <t>rel_abs_dif</t>
   </si>
   <si>
-    <t>DenseDepth_nohints</t>
-  </si>
-  <si>
-    <t>Uses rawdepth for evaluation (masks off invalid depth pixels), unlike what Wonka et.al. do in their paper.</t>
-  </si>
-  <si>
-    <t>Pytorch version. Will run caffe version soon.</t>
+    <t>DenseDepth</t>
+  </si>
+  <si>
+    <t>Evaluation: Ground truth depth is the inpainted depth cropped to 592x440 according to the official crop. RMSE is averaged across all RMSEs (rather than the square root of the average MSE)</t>
+  </si>
+  <si>
+    <t>DenseDepth (median rescaling)</t>
+  </si>
+  <si>
+    <t>DORN (median rescaling)</t>
+  </si>
+  <si>
+    <t>Matches what is published on github.</t>
+  </si>
+  <si>
+    <t>DORN (caffe)</t>
   </si>
 </sst>
 </file>
@@ -538,17 +547,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFB707D8-7A70-7644-B29D-168617A77793}">
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="55.5" customWidth="1"/>
     <col min="2" max="10" width="10.83203125" style="2"/>
-    <col min="12" max="12" width="39.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="62" style="1" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -627,7 +637,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -665,7 +675,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -703,7 +713,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -843,556 +853,529 @@
         <v>0.14955806691523499</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>38</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0.82799999999999996</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0.96499999999999997</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0.99199999999999999</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0.50900000000000001</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0.115</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="2">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B13" s="2">
-        <v>0.81100000000000005</v>
+        <v>0.82799999999999996</v>
       </c>
       <c r="C13" s="2">
-        <v>0.95299999999999996</v>
+        <v>0.96499999999999997</v>
       </c>
       <c r="D13" s="2">
-        <v>0.98799999999999999</v>
+        <v>0.99199999999999999</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F13" s="2">
-        <v>0.57299999999999995</v>
+        <v>0.50900000000000001</v>
       </c>
       <c r="G13" s="2">
-        <v>0.127</v>
+        <v>0.115</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I13" s="2">
-        <v>5.5E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="B14" s="2">
-        <v>0.84599999999999997</v>
+        <v>0.81100000000000005</v>
       </c>
       <c r="C14" s="2">
-        <v>0.97399999999999998</v>
+        <v>0.95299999999999996</v>
       </c>
       <c r="D14" s="2">
-        <v>0.99399999999999999</v>
+        <v>0.98799999999999999</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F14" s="2">
-        <v>0.46500000000000002</v>
+        <v>0.57299999999999995</v>
       </c>
       <c r="G14" s="2">
-        <v>0.123</v>
+        <v>0.127</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I14" s="2">
-        <v>5.2999999999999999E-2</v>
+        <v>5.5E-2</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="4">
-        <v>0.89500000000000002</v>
-      </c>
-      <c r="C15" s="4">
-        <v>0.98</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0.996</v>
+        <v>37</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.99399999999999999</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="4">
-        <v>0.39</v>
-      </c>
-      <c r="G15" s="4">
-        <v>0.10299999999999999</v>
+      <c r="F15" s="2">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.123</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="4">
-        <v>4.2999999999999997E-2</v>
+      <c r="I15" s="2">
+        <v>5.2999999999999999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.98</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.996</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0.39</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="4">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B17" s="2">
         <v>0.86599999999999999</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C17" s="2">
         <v>0.97499999999999998</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D17" s="2">
         <v>0.99299999999999999</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F17" s="2">
         <v>0.53</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G17" s="2">
         <v>0.115</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I17" s="2">
         <v>0.05</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="2">
-        <v>0.96081145008900004</v>
-      </c>
-      <c r="C21" s="2">
-        <v>0.98701898323668003</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0.993528499443877</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0.232361859312993</v>
-      </c>
-      <c r="F21" s="2">
-        <v>0.40572641363525003</v>
-      </c>
-      <c r="G21" s="4">
-        <v>5.7018968433220601E-2</v>
-      </c>
-      <c r="H21" s="2">
-        <v>7.0298137308973899E-2</v>
-      </c>
-      <c r="I21" s="4">
-        <v>2.40471564270456E-2</v>
-      </c>
-      <c r="J21" s="2">
-        <v>0.103031611054323</v>
+        <v>18</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="4">
-        <v>0.98305151418665204</v>
-      </c>
-      <c r="C22" s="4">
-        <v>0.99584115235829396</v>
-      </c>
-      <c r="D22" s="4">
-        <v>0.99860042441666297</v>
-      </c>
-      <c r="E22" s="4">
-        <v>0.109772951824067</v>
-      </c>
-      <c r="F22" s="4">
-        <v>0.294086728128932</v>
-      </c>
-      <c r="G22" s="2">
-        <v>7.6681173613611806E-2</v>
-      </c>
-      <c r="H22" s="4">
-        <v>2.8420280050566401E-2</v>
-      </c>
-      <c r="I22" s="2">
-        <v>3.4835308734914701E-2</v>
-      </c>
-      <c r="J22" s="4">
-        <v>9.6247356015322097E-2</v>
+        <v>19</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.96081145008900004</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.98701898323668003</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.993528499443877</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.232361859312993</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.40572641363525003</v>
+      </c>
+      <c r="G22" s="4">
+        <v>5.7018968433220601E-2</v>
+      </c>
+      <c r="H22" s="2">
+        <v>7.0298137308973899E-2</v>
+      </c>
+      <c r="I22" s="4">
+        <v>2.40471564270456E-2</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0.103031611054323</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0.98305151418665204</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.99584115235829396</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0.99860042441666297</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0.109772951824067</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0.294086728128932</v>
+      </c>
+      <c r="G23" s="2">
+        <v>7.6681173613611806E-2</v>
+      </c>
+      <c r="H23" s="4">
+        <v>2.8420280050566401E-2</v>
+      </c>
+      <c r="I23" s="2">
+        <v>3.4835308734914701E-2</v>
+      </c>
+      <c r="J23" s="4">
+        <v>9.6247356015322097E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B24" s="2">
         <v>0.97945953669757002</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C24" s="2">
         <v>0.994678041453117</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D24" s="2">
         <v>0.99806731906079904</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E24" s="2">
         <v>0.118581589964839</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F24" s="2">
         <v>0.30914099379332699</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G24" s="2">
         <v>8.4022855021325601E-2</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H24" s="2">
         <v>3.1475905720026003E-2</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I24" s="2">
         <v>3.8626020417079E-2</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J24" s="2">
         <v>0.105912321823124</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="25" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>29</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" s="4">
-        <v>0.89904221261380002</v>
-      </c>
-      <c r="C31" s="4">
-        <v>0.97003431706616206</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0.98950705422101004</v>
-      </c>
-      <c r="E31" s="4">
-        <v>0.327582259948069</v>
-      </c>
-      <c r="F31" s="4">
-        <v>0.49349046932983898</v>
-      </c>
-      <c r="G31" s="4">
-        <v>9.56505366146706E-2</v>
-      </c>
-      <c r="H31" s="2">
-        <v>9.5240771665649898E-2</v>
-      </c>
-      <c r="I31" s="4">
-        <v>4.1258352318578197E-2</v>
-      </c>
-      <c r="J31" s="4">
-        <v>0.14920161123915801</v>
+        <v>21</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32" s="2">
-        <v>0.841275141420047</v>
-      </c>
-      <c r="C32" s="2">
-        <v>0.96998454157297598</v>
-      </c>
-      <c r="D32" s="4">
-        <v>0.99213905857897899</v>
-      </c>
-      <c r="E32" s="2">
-        <v>0.329103093772459</v>
-      </c>
-      <c r="F32" s="2">
-        <v>0.50371245100018802</v>
-      </c>
-      <c r="G32" s="2">
-        <v>0.13229654983300401</v>
-      </c>
-      <c r="H32" s="4">
-        <v>8.8726245749514099E-2</v>
-      </c>
-      <c r="I32" s="2">
-        <v>5.9888827039364302E-2</v>
-      </c>
-      <c r="J32" s="2">
-        <v>0.17088902548313301</v>
+        <v>19</v>
+      </c>
+      <c r="B32" s="4">
+        <v>0.89904221261380002</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0.97003431706616206</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.98950705422101004</v>
+      </c>
+      <c r="E32" s="4">
+        <v>0.327582259948069</v>
+      </c>
+      <c r="F32" s="4">
+        <v>0.49349046932983898</v>
+      </c>
+      <c r="G32" s="4">
+        <v>9.56505366146706E-2</v>
+      </c>
+      <c r="H32" s="2">
+        <v>9.5240771665649898E-2</v>
+      </c>
+      <c r="I32" s="4">
+        <v>4.1258352318578197E-2</v>
+      </c>
+      <c r="J32" s="4">
+        <v>0.14920161123915801</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0.841275141420047</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.96998454157297598</v>
+      </c>
+      <c r="D33" s="4">
+        <v>0.99213905857897899</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0.329103093772459</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0.50371245100018802</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0.13229654983300401</v>
+      </c>
+      <c r="H33" s="4">
+        <v>8.8726245749514099E-2</v>
+      </c>
+      <c r="I33" s="2">
+        <v>5.9888827039364302E-2</v>
+      </c>
+      <c r="J33" s="2">
+        <v>0.17088902548313301</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B34" s="2">
         <v>0.81476784850522999</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C34" s="2">
         <v>0.96198267544571603</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D34" s="2">
         <v>0.98877794749748205</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E34" s="2">
         <v>0.35609781634842802</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F34" s="2">
         <v>0.52671933192250497</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G34" s="2">
         <v>0.14037138348744799</v>
       </c>
-      <c r="H33" s="2">
+      <c r="H34" s="2">
         <v>9.6165938413780502E-2</v>
       </c>
-      <c r="I33" s="2">
+      <c r="I34" s="2">
         <v>6.5396469234199894E-2</v>
       </c>
-      <c r="J33" s="2">
+      <c r="J34" s="2">
         <v>0.186160584261236</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="37" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B37" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C37" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D37" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F37" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G37" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="H37" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I36" s="2" t="s">
+      <c r="I37" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="J37" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>22</v>
-      </c>
-      <c r="B37" s="2">
-        <v>0.83929108669991404</v>
-      </c>
-      <c r="C37" s="2">
-        <v>0.95858464605035199</v>
-      </c>
-      <c r="D37" s="2">
-        <v>0.98564354107743601</v>
-      </c>
-      <c r="E37" s="2">
-        <v>0.26140680609123301</v>
-      </c>
-      <c r="F37" s="2">
-        <f>SQRT(E37)</f>
-        <v>0.51127957722877315</v>
-      </c>
-      <c r="G37" s="2">
-        <v>0.12950759483657001</v>
-      </c>
-      <c r="H37" s="2">
-        <v>8.7568223680133297E-2</v>
-      </c>
-      <c r="I37" s="2">
-        <v>5.8503517225143298E-2</v>
-      </c>
-      <c r="J37" s="2">
-        <v>0.17285743104927601</v>
-      </c>
       <c r="L37" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="2">
+        <v>0.84709999999999996</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0.97309999999999997</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.99370000000000003</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0.46110000000000001</v>
+      </c>
+      <c r="G43" s="2">
+        <v>0.1234</v>
+      </c>
+      <c r="I43" s="2">
+        <v>5.3499999999999999E-2</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38" s="2">
-        <v>0.85618639232578697</v>
-      </c>
-      <c r="C38" s="2">
-        <v>0.97836328187102095</v>
-      </c>
-      <c r="D38" s="2">
-        <v>0.99565340722963402</v>
-      </c>
-      <c r="E38" s="2">
-        <v>0.21353111323962001</v>
-      </c>
-      <c r="F38" s="2">
-        <f>SQRT(E38)</f>
-        <v>0.4620942687803215</v>
-      </c>
-      <c r="G38" s="2">
-        <v>0.11950074903631699</v>
-      </c>
-      <c r="H38" s="2">
-        <v>6.8724721778946202E-2</v>
-      </c>
-      <c r="I38" s="2">
-        <v>5.1383407905070101E-2</v>
-      </c>
-      <c r="J38" s="2">
-        <v>0.151374158361015</v>
-      </c>
-      <c r="L38" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
+    <row r="45" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Filled out middle section of table, even though it doesn't match published work.
</commit_message>
<xml_diff>
--- a/paper/DepthNet.xlsx
+++ b/paper/DepthNet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Documents/Stanford/ares/spad_single/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A5E402-A504-B249-B436-9C705D1309F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151CCA83-DF66-EA4E-8972-11696F5C4FA4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5420" yWindow="1480" windowWidth="28800" windowHeight="17540" xr2:uid="{777694D5-0BD5-8249-BEEC-1B33D94A54A3}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="55">
   <si>
     <t>DORN</t>
   </si>
@@ -178,7 +178,19 @@
     <t>Matches what is published on github.</t>
   </si>
   <si>
-    <t>DORN (caffe)</t>
+    <t>Does not match what is published</t>
+  </si>
+  <si>
+    <t>DORN (GT histogram matching)</t>
+  </si>
+  <si>
+    <t>DenseDepth (GT histogram matching)</t>
+  </si>
+  <si>
+    <t>DORN (pytorch)</t>
+  </si>
+  <si>
+    <t>DORN evaluation doesn't match but whatever</t>
   </si>
 </sst>
 </file>
@@ -549,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFB707D8-7A70-7644-B29D-168617A77793}">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1334,15 +1346,77 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>53</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.95420000000000005</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.98270000000000002</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0.50070000000000003</v>
+      </c>
+      <c r="G38" s="2">
+        <v>0.1197</v>
+      </c>
+      <c r="I38" s="2">
+        <v>5.33E-2</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>48</v>
       </c>
+      <c r="B39" s="2">
+        <v>0.86829999999999996</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0.96419999999999995</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.98850000000000005</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0.48380000000000001</v>
+      </c>
+      <c r="G39" s="2">
+        <v>0.11509999999999999</v>
+      </c>
+      <c r="I39" s="2">
+        <v>4.9299999999999997E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="2">
+        <v>0.9022</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.99050000000000005</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0.42359999999999998</v>
+      </c>
+      <c r="G40" s="2">
+        <v>9.9299999999999999E-2</v>
+      </c>
+      <c r="I40" s="2">
+        <v>4.1700000000000001E-2</v>
+      </c>
     </row>
     <row r="43" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
@@ -1374,8 +1448,51 @@
       <c r="A44" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B44" s="2">
+        <v>0.88759999999999994</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.9778</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.99519999999999997</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0.40910000000000002</v>
+      </c>
+      <c r="G44" s="2">
+        <v>0.106</v>
+      </c>
+      <c r="I44" s="2">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="2">
+        <v>0.92949999999999999</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0.99539999999999995</v>
+      </c>
+      <c r="F45" s="2">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="G45" s="2">
+        <v>8.0299999999999996E-2</v>
+      </c>
+      <c r="I45" s="2">
+        <v>3.4200000000000001E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New file structure, setup.py, finished new weighted histogram matching method.
</commit_message>
<xml_diff>
--- a/paper/DepthNet.xlsx
+++ b/paper/DepthNet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Documents/Stanford/ares/spad_single/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151CCA83-DF66-EA4E-8972-11696F5C4FA4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E0A779-B3B9-0841-A304-472A2BFC86E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5420" yWindow="1480" windowWidth="28800" windowHeight="17540" xr2:uid="{777694D5-0BD5-8249-BEEC-1B33D94A54A3}"/>
+    <workbookView xWindow="19140" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{777694D5-0BD5-8249-BEEC-1B33D94A54A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="57">
   <si>
     <t>DORN</t>
   </si>
@@ -178,9 +178,6 @@
     <t>Matches what is published on github.</t>
   </si>
   <si>
-    <t>Does not match what is published</t>
-  </si>
-  <si>
     <t>DORN (GT histogram matching)</t>
   </si>
   <si>
@@ -191,6 +188,15 @@
   </si>
   <si>
     <t>DORN evaluation doesn't match but whatever</t>
+  </si>
+  <si>
+    <t>Does not match what is published: UPDATE: Because github model is close but not quite as good as what went in the paper.</t>
+  </si>
+  <si>
+    <t>DenseDepth (Wasserstein histogram matching)</t>
+  </si>
+  <si>
+    <t>DORN (Wasserstein histogram matching)</t>
   </si>
 </sst>
 </file>
@@ -559,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFB707D8-7A70-7644-B29D-168617A77793}">
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1348,7 +1354,7 @@
     </row>
     <row r="38" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B38" s="2">
         <v>0.84599999999999997</v>
@@ -1369,7 +1375,7 @@
         <v>5.33E-2</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
@@ -1397,7 +1403,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B40" s="2">
         <v>0.9022</v>
@@ -1416,6 +1422,29 @@
       </c>
       <c r="I40" s="2">
         <v>4.1700000000000001E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41" s="2">
+        <v>0.847427449419342</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.95332383895321304</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.982672920285379</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0.49932645306856899</v>
+      </c>
+      <c r="G41" s="2">
+        <v>0.117189220622728</v>
+      </c>
+      <c r="I41" s="2">
+        <v>5.3489108434636203E-2</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1444,7 +1473,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -1467,12 +1496,12 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B45" s="2">
         <v>0.92949999999999999</v>
@@ -1491,6 +1520,11 @@
       </c>
       <c r="I45" s="2">
         <v>3.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DORN with weighted histogram matching works.
</commit_message>
<xml_diff>
--- a/paper/DepthNet.xlsx
+++ b/paper/DepthNet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Documents/Stanford/ares/spad_single/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E0A779-B3B9-0841-A304-472A2BFC86E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3E0838-6AD6-CE40-A471-993404D8CC0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19140" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{777694D5-0BD5-8249-BEEC-1B33D94A54A3}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{777694D5-0BD5-8249-BEEC-1B33D94A54A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="63">
   <si>
     <t>DORN</t>
   </si>
@@ -197,6 +197,24 @@
   </si>
   <si>
     <t>DORN (Wasserstein histogram matching)</t>
+  </si>
+  <si>
+    <t>DORN (Weighted histogram matching)</t>
+  </si>
+  <si>
+    <t>Intensity Only</t>
+  </si>
+  <si>
+    <t>Intensity and Falloff</t>
+  </si>
+  <si>
+    <t>Intensity, Falloff, and DC/Ambient</t>
+  </si>
+  <si>
+    <t>Intensity, Falloff, DC/Ambient, and Jitter</t>
+  </si>
+  <si>
+    <t>Intensity, Falloff, DC/Ambient, Jitter, and Poisson Noise</t>
   </si>
 </sst>
 </file>
@@ -565,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFB707D8-7A70-7644-B29D-168617A77793}">
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J45" sqref="J45"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:XFD52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1447,83 +1465,213 @@
         <v>5.3489108434636203E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43" s="2">
+        <v>0.90449999999999997</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0.97050000000000003</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.98919999999999997</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0.41420000000000001</v>
+      </c>
+      <c r="G43" s="2">
+        <v>9.1200000000000003E-2</v>
+      </c>
+      <c r="I43" s="2">
+        <v>3.95E-2</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" s="2">
+        <v>0.90449999999999997</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.97050000000000003</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.98919999999999997</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0.4143</v>
+      </c>
+      <c r="G44" s="2">
+        <v>9.1200000000000003E-2</v>
+      </c>
+      <c r="I44" s="2">
+        <v>3.95E-2</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>57</v>
+      </c>
+      <c r="B45" s="2">
+        <v>0.90410000000000001</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0.97</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0.9889</v>
+      </c>
+      <c r="F45" s="2">
+        <v>0.4173</v>
+      </c>
+      <c r="G45" s="2">
+        <v>9.0200000000000002E-2</v>
+      </c>
+      <c r="I45" s="2">
+        <v>3.9600000000000003E-2</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" s="2">
+        <v>0.90410000000000001</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0.97009999999999996</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0.9889</v>
+      </c>
+      <c r="F46" s="2">
+        <v>0.4168</v>
+      </c>
+      <c r="G46" s="2">
+        <v>9.0300000000000005E-2</v>
+      </c>
+      <c r="I46" s="2">
+        <v>3.9600000000000003E-2</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>57</v>
+      </c>
+      <c r="B47" s="2">
+        <v>0.90310000000000001</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0.96909999999999996</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0.98809999999999998</v>
+      </c>
+      <c r="F47" s="2">
+        <v>0.45860000000000001</v>
+      </c>
+      <c r="G47" s="2">
+        <v>9.2600000000000002E-2</v>
+      </c>
+      <c r="I47" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B49" s="2">
         <v>0.84709999999999996</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C49" s="2">
         <v>0.97309999999999997</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D49" s="2">
         <v>0.99370000000000003</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F49" s="2">
         <v>0.46110000000000001</v>
       </c>
-      <c r="G43" s="2">
+      <c r="G49" s="2">
         <v>0.1234</v>
       </c>
-      <c r="I43" s="2">
+      <c r="I49" s="2">
         <v>5.3499999999999999E-2</v>
       </c>
-      <c r="L43" s="1" t="s">
+      <c r="L49" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="50" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B50" s="2">
         <v>0.88759999999999994</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C50" s="2">
         <v>0.9778</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D50" s="2">
         <v>0.99519999999999997</v>
       </c>
-      <c r="F44" s="2">
+      <c r="F50" s="2">
         <v>0.40910000000000002</v>
       </c>
-      <c r="G44" s="2">
+      <c r="G50" s="2">
         <v>0.106</v>
       </c>
-      <c r="I44" s="2">
+      <c r="I50" s="2">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="L44" s="1" t="s">
+      <c r="L50" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="51" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B51" s="2">
         <v>0.92949999999999999</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C51" s="2">
         <v>0.98399999999999999</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D51" s="2">
         <v>0.99539999999999995</v>
       </c>
-      <c r="F45" s="2">
+      <c r="F51" s="2">
         <v>0.33800000000000002</v>
       </c>
-      <c r="G45" s="2">
+      <c r="G51" s="2">
         <v>8.0299999999999996E-2</v>
       </c>
-      <c r="I45" s="2">
+      <c r="I51" s="2">
         <v>3.4200000000000001E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Evaluating weighted histogram matching with DenseDepth.
</commit_message>
<xml_diff>
--- a/paper/DepthNet.xlsx
+++ b/paper/DepthNet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Documents/Stanford/ares/spad_single/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3E0838-6AD6-CE40-A471-993404D8CC0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7268B947-C2CB-CE41-88C9-C3516C415AB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{777694D5-0BD5-8249-BEEC-1B33D94A54A3}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="63">
   <si>
     <t>DORN</t>
   </si>
@@ -193,9 +193,6 @@
     <t>Does not match what is published: UPDATE: Because github model is close but not quite as good as what went in the paper.</t>
   </si>
   <si>
-    <t>DenseDepth (Wasserstein histogram matching)</t>
-  </si>
-  <si>
     <t>DORN (Wasserstein histogram matching)</t>
   </si>
   <si>
@@ -215,6 +212,9 @@
   </si>
   <si>
     <t>Intensity, Falloff, DC/Ambient, Jitter, and Poisson Noise</t>
+  </si>
+  <si>
+    <t>DenseDepth (Weighted histogram matching)</t>
   </si>
 </sst>
 </file>
@@ -583,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFB707D8-7A70-7644-B29D-168617A77793}">
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:XFD52"/>
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1444,7 +1444,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B41" s="2">
         <v>0.847427449419342</v>
@@ -1467,7 +1467,7 @@
     </row>
     <row r="43" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B43" s="2">
         <v>0.90449999999999997</v>
@@ -1488,12 +1488,12 @@
         <v>3.95E-2</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B44" s="2">
         <v>0.90449999999999997</v>
@@ -1514,12 +1514,12 @@
         <v>3.95E-2</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B45" s="2">
         <v>0.90410000000000001</v>
@@ -1540,12 +1540,12 @@
         <v>3.9600000000000003E-2</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B46" s="2">
         <v>0.90410000000000001</v>
@@ -1566,12 +1566,12 @@
         <v>3.9600000000000003E-2</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B47" s="2">
         <v>0.90310000000000001</v>
@@ -1592,7 +1592,7 @@
         <v>0.04</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1670,9 +1670,12 @@
         <v>3.4200000000000001E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>55</v>
+    <row r="53" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>62</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Poisson denoising with rmse=0.373
</commit_message>
<xml_diff>
--- a/paper/DepthNet.xlsx
+++ b/paper/DepthNet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Documents/Stanford/ares/spad_single/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7268B947-C2CB-CE41-88C9-C3516C415AB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F256438-A14E-2F4A-9E67-8995E90CD50B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{777694D5-0BD5-8249-BEEC-1B33D94A54A3}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="68">
   <si>
     <t>DORN</t>
   </si>
@@ -215,6 +215,21 @@
   </si>
   <si>
     <t>DenseDepth (Weighted histogram matching)</t>
+  </si>
+  <si>
+    <t>lam=1e-2</t>
+  </si>
+  <si>
+    <t>lam-1e-2</t>
+  </si>
+  <si>
+    <t>lam=1e1</t>
+  </si>
+  <si>
+    <t>Intensity Only (Poissn Denoising) (sid_bins=140) (lam=1e0)</t>
+  </si>
+  <si>
+    <t>Intensity, Falloff, DC/Ambient, Jitter, and Poisson Noise (Poisson Denoising) (sid_bins=140) (lam=1e0)</t>
   </si>
 </sst>
 </file>
@@ -583,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFB707D8-7A70-7644-B29D-168617A77793}">
-  <dimension ref="A1:M53"/>
+  <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="B37" zoomScale="107" zoomScaleNormal="143" workbookViewId="0">
+      <selection activeCell="L60" sqref="L60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1595,7 +1610,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>45</v>
       </c>
@@ -1621,7 +1636,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -1647,7 +1662,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -1670,12 +1685,183 @@
         <v>3.4200000000000001E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>62</v>
       </c>
+      <c r="B53" s="2">
+        <v>0.92390000000000005</v>
+      </c>
+      <c r="C53" s="2">
+        <v>0.98250000000000004</v>
+      </c>
+      <c r="D53" s="2">
+        <v>0.99439999999999995</v>
+      </c>
+      <c r="F53" s="2">
+        <v>0.35520000000000002</v>
+      </c>
+      <c r="G53" s="2">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="I53" s="2">
+        <v>3.5999999999999997E-2</v>
+      </c>
       <c r="L53" s="1" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54" s="2">
+        <v>0.92390000000000005</v>
+      </c>
+      <c r="C54" s="2">
+        <v>0.98250000000000004</v>
+      </c>
+      <c r="D54" s="2">
+        <v>0.99439999999999995</v>
+      </c>
+      <c r="F54" s="2">
+        <v>0.35520000000000002</v>
+      </c>
+      <c r="G54" s="2">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="I54" s="2">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" s="2">
+        <v>0.92379999999999995</v>
+      </c>
+      <c r="C55" s="2">
+        <v>0.98270000000000002</v>
+      </c>
+      <c r="D55" s="2">
+        <v>0.99470000000000003</v>
+      </c>
+      <c r="F55" s="2">
+        <v>0.35449999999999998</v>
+      </c>
+      <c r="G55" s="2">
+        <v>8.3599999999999994E-2</v>
+      </c>
+      <c r="I55" s="2">
+        <v>3.5799999999999998E-2</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M55" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>62</v>
+      </c>
+      <c r="B56" s="2">
+        <v>0.92390000000000005</v>
+      </c>
+      <c r="C56" s="2">
+        <v>0.98280000000000001</v>
+      </c>
+      <c r="D56" s="2">
+        <v>0.99470000000000003</v>
+      </c>
+      <c r="F56" s="2">
+        <v>0.35349999999999998</v>
+      </c>
+      <c r="G56" s="2">
+        <v>8.3599999999999994E-2</v>
+      </c>
+      <c r="I56" s="2">
+        <v>3.5799999999999998E-2</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M56" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" s="2">
+        <v>0.92120000000000002</v>
+      </c>
+      <c r="C57" s="2">
+        <v>0.98109999999999997</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0.99360000000000004</v>
+      </c>
+      <c r="F57" s="2">
+        <v>0.3947</v>
+      </c>
+      <c r="G57" s="2">
+        <v>8.5900000000000004E-2</v>
+      </c>
+      <c r="I57" s="2">
+        <v>3.6600000000000001E-2</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M57" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59" s="2">
+        <v>0.92589999999999995</v>
+      </c>
+      <c r="F59" s="2">
+        <v>0.34470000000000001</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60" s="2">
+        <v>0.92059999999999997</v>
+      </c>
+      <c r="C60" s="2">
+        <v>0.98119999999999996</v>
+      </c>
+      <c r="D60" s="2">
+        <v>0.99390000000000001</v>
+      </c>
+      <c r="F60" s="2">
+        <v>0.37259999999999999</v>
+      </c>
+      <c r="G60" s="2">
+        <v>8.5900000000000004E-2</v>
+      </c>
+      <c r="I60" s="2">
+        <v>3.6600000000000001E-2</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated config to match optimal results.
</commit_message>
<xml_diff>
--- a/paper/DepthNet.xlsx
+++ b/paper/DepthNet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Documents/Stanford/ares/spad_single/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F256438-A14E-2F4A-9E67-8995E90CD50B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1648DDD2-FA43-0648-B148-C7323C19D0FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{777694D5-0BD5-8249-BEEC-1B33D94A54A3}"/>
+    <workbookView xWindow="38400" yWindow="-19000" windowWidth="21600" windowHeight="37940" xr2:uid="{777694D5-0BD5-8249-BEEC-1B33D94A54A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
@@ -226,10 +226,10 @@
     <t>lam=1e1</t>
   </si>
   <si>
-    <t>Intensity Only (Poissn Denoising) (sid_bins=140) (lam=1e0)</t>
-  </si>
-  <si>
-    <t>Intensity, Falloff, DC/Ambient, Jitter, and Poisson Noise (Poisson Denoising) (sid_bins=140) (lam=1e0)</t>
+    <t>Intensity, Falloff, DC/Ambient, Jitter, and Poisson Noise (Poisson Denoising) (sid_bins=140) (lam=1e1)</t>
+  </si>
+  <si>
+    <t>Intensity Only (sid_bins=140)</t>
   </si>
 </sst>
 </file>
@@ -600,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFB707D8-7A70-7644-B29D-168617A77793}">
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" zoomScale="107" zoomScaleNormal="143" workbookViewId="0">
-      <selection activeCell="L60" sqref="L60"/>
+    <sheetView tabSelected="1" topLeftCell="C37" zoomScale="107" zoomScaleNormal="143" workbookViewId="0">
+      <selection activeCell="L59" sqref="L59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1831,11 +1831,23 @@
       <c r="B59" s="2">
         <v>0.92589999999999995</v>
       </c>
+      <c r="C59" s="2">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="D59" s="2">
+        <v>0.99480000000000002</v>
+      </c>
       <c r="F59" s="2">
         <v>0.34470000000000001</v>
       </c>
+      <c r="G59" s="2">
+        <v>8.0799999999999997E-2</v>
+      </c>
+      <c r="I59" s="2">
+        <v>3.4700000000000002E-2</v>
+      </c>
       <c r="L59" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="34" x14ac:dyDescent="0.2">
@@ -1861,11 +1873,12 @@
         <v>3.6600000000000001E-2</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Wavelet Denoising, then dc removal.
</commit_message>
<xml_diff>
--- a/paper/DepthNet.xlsx
+++ b/paper/DepthNet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Documents/Stanford/ares/spad_single/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1648DDD2-FA43-0648-B148-C7323C19D0FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7B69AE-DA84-0946-AB45-DFB4A391003A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="-19000" windowWidth="21600" windowHeight="37940" xr2:uid="{777694D5-0BD5-8249-BEEC-1B33D94A54A3}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{777694D5-0BD5-8249-BEEC-1B33D94A54A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
@@ -600,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFB707D8-7A70-7644-B29D-168617A77793}">
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C37" zoomScale="107" zoomScaleNormal="143" workbookViewId="0">
-      <selection activeCell="L59" sqref="L59"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="107" zoomScaleNormal="143" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1829,22 +1829,22 @@
         <v>62</v>
       </c>
       <c r="B59" s="2">
-        <v>0.92589999999999995</v>
+        <v>0.92549999999999999</v>
       </c>
       <c r="C59" s="2">
-        <v>0.98299999999999998</v>
+        <v>0.9829</v>
       </c>
       <c r="D59" s="2">
         <v>0.99480000000000002</v>
       </c>
       <c r="F59" s="2">
-        <v>0.34470000000000001</v>
+        <v>0.34599999999999997</v>
       </c>
       <c r="G59" s="2">
-        <v>8.0799999999999997E-2</v>
+        <v>8.1299999999999997E-2</v>
       </c>
       <c r="I59" s="2">
-        <v>3.4700000000000002E-2</v>
+        <v>3.49E-2</v>
       </c>
       <c r="L59" s="1" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
Median matching and gt hist matching, plus table draft 1.
</commit_message>
<xml_diff>
--- a/paper/DepthNet.xlsx
+++ b/paper/DepthNet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Documents/Stanford/ares/spad_single/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7B69AE-DA84-0946-AB45-DFB4A391003A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A6EA77-8A86-7C4B-A23C-17F1F1337BC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{777694D5-0BD5-8249-BEEC-1B33D94A54A3}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="34660" windowHeight="17540" xr2:uid="{777694D5-0BD5-8249-BEEC-1B33D94A54A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="69">
   <si>
     <t>DORN</t>
   </si>
@@ -226,10 +226,13 @@
     <t>lam=1e1</t>
   </si>
   <si>
-    <t>Intensity, Falloff, DC/Ambient, Jitter, and Poisson Noise (Poisson Denoising) (sid_bins=140) (lam=1e1)</t>
-  </si>
-  <si>
-    <t>Intensity Only (sid_bins=140)</t>
+    <t>SBR = 10</t>
+  </si>
+  <si>
+    <t>SBR = 50</t>
+  </si>
+  <si>
+    <t>SBR = 100</t>
   </si>
 </sst>
 </file>
@@ -256,12 +259,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -276,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -284,6 +293,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFB707D8-7A70-7644-B29D-168617A77793}">
-  <dimension ref="A1:M60"/>
+  <dimension ref="A1:M63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" zoomScale="107" zoomScaleNormal="143" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+      <selection activeCell="A41" sqref="A41:XFD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1286,7 +1300,7 @@
         <v>0.14920161123915801</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>20</v>
       </c>
@@ -1318,7 +1332,7 @@
         <v>0.17088902548313301</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -1350,7 +1364,7 @@
         <v>0.186160584261236</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -1385,7 +1399,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -1411,53 +1425,53 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>48</v>
       </c>
       <c r="B39" s="2">
-        <v>0.86829999999999996</v>
+        <v>0.87129999999999996</v>
       </c>
       <c r="C39" s="2">
-        <v>0.96419999999999995</v>
+        <v>0.96399999999999997</v>
       </c>
       <c r="D39" s="2">
-        <v>0.98850000000000005</v>
+        <v>0.98809999999999998</v>
       </c>
       <c r="F39" s="2">
-        <v>0.48380000000000001</v>
+        <v>0.47299999999999998</v>
       </c>
       <c r="G39" s="2">
-        <v>0.11509999999999999</v>
+        <v>0.1108</v>
       </c>
       <c r="I39" s="2">
-        <v>4.9299999999999997E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+        <v>4.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>50</v>
       </c>
       <c r="B40" s="2">
-        <v>0.9022</v>
+        <v>0.90620000000000001</v>
       </c>
       <c r="C40" s="2">
-        <v>0.97299999999999998</v>
+        <v>0.97240000000000004</v>
       </c>
       <c r="D40" s="2">
-        <v>0.99050000000000005</v>
+        <v>0.99029999999999996</v>
       </c>
       <c r="F40" s="2">
-        <v>0.42359999999999998</v>
+        <v>0.4194</v>
       </c>
       <c r="G40" s="2">
-        <v>9.9299999999999999E-2</v>
+        <v>9.4899999999999998E-2</v>
       </c>
       <c r="I40" s="2">
-        <v>4.1700000000000001E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+        <v>4.02E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -1480,7 +1494,7 @@
         <v>5.3489108434636203E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>56</v>
       </c>
@@ -1506,264 +1520,286 @@
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="44" spans="1:13" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="6">
         <v>0.90449999999999997</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="6">
         <v>0.97050000000000003</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44" s="6">
         <v>0.98919999999999997</v>
       </c>
-      <c r="F44" s="2">
+      <c r="E44" s="6"/>
+      <c r="F44" s="6">
         <v>0.4143</v>
       </c>
-      <c r="G44" s="2">
+      <c r="G44" s="6">
         <v>9.1200000000000003E-2</v>
       </c>
-      <c r="I44" s="2">
+      <c r="H44" s="6"/>
+      <c r="I44" s="6">
         <v>3.95E-2</v>
       </c>
-      <c r="L44" s="1" t="s">
+      <c r="J44" s="6"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="45" spans="1:13" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="6">
         <v>0.90410000000000001</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="6">
         <v>0.97</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D45" s="6">
         <v>0.9889</v>
       </c>
-      <c r="F45" s="2">
+      <c r="E45" s="6"/>
+      <c r="F45" s="6">
         <v>0.4173</v>
       </c>
-      <c r="G45" s="2">
+      <c r="G45" s="6">
         <v>9.0200000000000002E-2</v>
       </c>
-      <c r="I45" s="2">
+      <c r="H45" s="6"/>
+      <c r="I45" s="6">
         <v>3.9600000000000003E-2</v>
       </c>
-      <c r="L45" s="1" t="s">
+      <c r="J45" s="6"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="46" spans="1:13" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46" s="6">
         <v>0.90410000000000001</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="6">
         <v>0.97009999999999996</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D46" s="6">
         <v>0.9889</v>
       </c>
-      <c r="F46" s="2">
+      <c r="E46" s="6"/>
+      <c r="F46" s="6">
         <v>0.4168</v>
       </c>
-      <c r="G46" s="2">
+      <c r="G46" s="6">
         <v>9.0300000000000005E-2</v>
       </c>
-      <c r="I46" s="2">
+      <c r="H46" s="6"/>
+      <c r="I46" s="6">
         <v>3.9600000000000003E-2</v>
       </c>
-      <c r="L46" s="1" t="s">
+      <c r="J46" s="6"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="47" spans="1:13" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="6">
         <v>0.90310000000000001</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="6">
         <v>0.96909999999999996</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D47" s="6">
         <v>0.98809999999999998</v>
       </c>
-      <c r="F47" s="2">
+      <c r="E47" s="6"/>
+      <c r="F47" s="6">
         <v>0.45860000000000001</v>
       </c>
-      <c r="G47" s="2">
+      <c r="G47" s="6">
         <v>9.2600000000000002E-2</v>
       </c>
-      <c r="I47" s="2">
+      <c r="H47" s="6"/>
+      <c r="I47" s="6">
         <v>0.04</v>
       </c>
-      <c r="L47" s="1" t="s">
+      <c r="J47" s="6"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48" s="2">
+        <v>0.90310000000000001</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0.97</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0.9889</v>
+      </c>
+      <c r="F48" s="2">
+        <v>0.42180000000000001</v>
+      </c>
+      <c r="G48" s="2">
+        <v>9.0899999999999995E-2</v>
+      </c>
+      <c r="I48" s="3">
+        <v>3.9899999999999998E-2</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M48" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" s="2">
+        <v>0.90569999999999995</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0.97109999999999996</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0.98960000000000004</v>
+      </c>
+      <c r="F49" s="2">
+        <v>0.40960000000000002</v>
+      </c>
+      <c r="G49" s="2">
+        <v>8.9399999999999993E-2</v>
+      </c>
+      <c r="I49" s="2">
+        <v>3.9100000000000003E-2</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M49" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>56</v>
+      </c>
+      <c r="B50" s="2">
+        <v>0.90629999999999999</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0.97140000000000004</v>
+      </c>
+      <c r="D50" s="2">
+        <v>0.98980000000000001</v>
+      </c>
+      <c r="F50" s="2">
+        <v>0.40810000000000002</v>
+      </c>
+      <c r="G50" s="2">
+        <v>8.9599999999999999E-2</v>
+      </c>
+      <c r="I50" s="2">
+        <v>3.8899999999999997E-2</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M50" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>45</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B52" s="2">
         <v>0.84709999999999996</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C52" s="2">
         <v>0.97309999999999997</v>
       </c>
-      <c r="D49" s="2">
+      <c r="D52" s="2">
         <v>0.99370000000000003</v>
       </c>
-      <c r="F49" s="2">
+      <c r="F52" s="2">
         <v>0.46110000000000001</v>
       </c>
-      <c r="G49" s="2">
+      <c r="G52" s="2">
         <v>0.1234</v>
       </c>
-      <c r="I49" s="2">
+      <c r="I52" s="2">
         <v>5.3499999999999999E-2</v>
       </c>
-      <c r="L49" s="1" t="s">
+      <c r="L52" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="53" spans="1:13" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>47</v>
       </c>
-      <c r="B50" s="2">
-        <v>0.88759999999999994</v>
-      </c>
-      <c r="C50" s="2">
-        <v>0.9778</v>
-      </c>
-      <c r="D50" s="2">
+      <c r="B53" s="2">
+        <v>0.88829999999999998</v>
+      </c>
+      <c r="C53" s="2">
+        <v>0.97760000000000002</v>
+      </c>
+      <c r="D53" s="2">
+        <v>0.99490000000000001</v>
+      </c>
+      <c r="F53" s="2">
+        <v>0.4093</v>
+      </c>
+      <c r="G53" s="2">
+        <v>0.10589999999999999</v>
+      </c>
+      <c r="I53" s="2">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>51</v>
+      </c>
+      <c r="B54" s="2">
+        <v>0.93010000000000004</v>
+      </c>
+      <c r="C54" s="2">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="D54" s="2">
         <v>0.99519999999999997</v>
       </c>
-      <c r="F50" s="2">
-        <v>0.40910000000000002</v>
-      </c>
-      <c r="G50" s="2">
-        <v>0.106</v>
-      </c>
-      <c r="I50" s="2">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="L50" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>51</v>
-      </c>
-      <c r="B51" s="2">
-        <v>0.92949999999999999</v>
-      </c>
-      <c r="C51" s="2">
-        <v>0.98399999999999999</v>
-      </c>
-      <c r="D51" s="2">
-        <v>0.99539999999999995</v>
-      </c>
-      <c r="F51" s="2">
-        <v>0.33800000000000002</v>
-      </c>
-      <c r="G51" s="2">
-        <v>8.0299999999999996E-2</v>
-      </c>
-      <c r="I51" s="2">
-        <v>3.4200000000000001E-2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>62</v>
-      </c>
-      <c r="B53" s="2">
-        <v>0.92390000000000005</v>
-      </c>
-      <c r="C53" s="2">
-        <v>0.98250000000000004</v>
-      </c>
-      <c r="D53" s="2">
-        <v>0.99439999999999995</v>
-      </c>
-      <c r="F53" s="2">
-        <v>0.35520000000000002</v>
-      </c>
-      <c r="G53" s="2">
-        <v>8.4000000000000005E-2</v>
-      </c>
-      <c r="I53" s="2">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="L53" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>62</v>
-      </c>
-      <c r="B54" s="2">
-        <v>0.92390000000000005</v>
-      </c>
-      <c r="C54" s="2">
-        <v>0.98250000000000004</v>
-      </c>
-      <c r="D54" s="2">
-        <v>0.99439999999999995</v>
-      </c>
       <c r="F54" s="2">
-        <v>0.35520000000000002</v>
+        <v>0.3377</v>
       </c>
       <c r="G54" s="2">
-        <v>8.4000000000000005E-2</v>
+        <v>7.9299999999999995E-2</v>
       </c>
       <c r="I54" s="2">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="L54" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>62</v>
-      </c>
-      <c r="B55" s="2">
-        <v>0.92379999999999995</v>
-      </c>
-      <c r="C55" s="2">
-        <v>0.98270000000000002</v>
-      </c>
-      <c r="D55" s="2">
-        <v>0.99470000000000003</v>
-      </c>
-      <c r="F55" s="2">
-        <v>0.35449999999999998</v>
-      </c>
-      <c r="G55" s="2">
-        <v>8.3599999999999994E-2</v>
-      </c>
-      <c r="I55" s="2">
-        <v>3.5799999999999998E-2</v>
-      </c>
-      <c r="L55" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="M55" t="s">
-        <v>64</v>
+        <v>3.39E-2</v>
       </c>
     </row>
     <row r="56" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -1774,106 +1810,234 @@
         <v>0.92390000000000005</v>
       </c>
       <c r="C56" s="2">
+        <v>0.98250000000000004</v>
+      </c>
+      <c r="D56" s="2">
+        <v>0.99439999999999995</v>
+      </c>
+      <c r="F56" s="2">
+        <v>0.35520000000000002</v>
+      </c>
+      <c r="G56" s="2">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="I56" s="2">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" s="5" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" s="6">
+        <v>0.92390000000000005</v>
+      </c>
+      <c r="C57" s="6">
+        <v>0.98250000000000004</v>
+      </c>
+      <c r="D57" s="6">
+        <v>0.99439999999999995</v>
+      </c>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6">
+        <v>0.35520000000000002</v>
+      </c>
+      <c r="G57" s="6">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="J57" s="6"/>
+      <c r="L57" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" s="5" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B58" s="6">
+        <v>0.92379999999999995</v>
+      </c>
+      <c r="C58" s="6">
+        <v>0.98270000000000002</v>
+      </c>
+      <c r="D58" s="6">
+        <v>0.99470000000000003</v>
+      </c>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6">
+        <v>0.35449999999999998</v>
+      </c>
+      <c r="G58" s="6">
+        <v>8.3599999999999994E-2</v>
+      </c>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6">
+        <v>3.5799999999999998E-2</v>
+      </c>
+      <c r="J58" s="6"/>
+      <c r="L58" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="M58" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" s="5" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59" s="6">
+        <v>0.92390000000000005</v>
+      </c>
+      <c r="C59" s="6">
         <v>0.98280000000000001</v>
       </c>
-      <c r="D56" s="2">
+      <c r="D59" s="6">
         <v>0.99470000000000003</v>
       </c>
-      <c r="F56" s="2">
+      <c r="E59" s="6"/>
+      <c r="F59" s="6">
         <v>0.35349999999999998</v>
       </c>
-      <c r="G56" s="2">
+      <c r="G59" s="6">
         <v>8.3599999999999994E-2</v>
       </c>
-      <c r="I56" s="2">
+      <c r="H59" s="6"/>
+      <c r="I59" s="6">
         <v>3.5799999999999998E-2</v>
       </c>
-      <c r="L56" s="1" t="s">
+      <c r="J59" s="6"/>
+      <c r="L59" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="M56" t="s">
+      <c r="M59" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="60" spans="1:13" s="5" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B60" s="6">
         <v>0.92120000000000002</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C60" s="6">
         <v>0.98109999999999997</v>
       </c>
-      <c r="D57" s="2">
+      <c r="D60" s="6">
         <v>0.99360000000000004</v>
       </c>
-      <c r="F57" s="2">
+      <c r="E60" s="6"/>
+      <c r="F60" s="6">
         <v>0.3947</v>
       </c>
-      <c r="G57" s="2">
+      <c r="G60" s="6">
         <v>8.5900000000000004E-2</v>
       </c>
-      <c r="I57" s="2">
+      <c r="H60" s="6"/>
+      <c r="I60" s="6">
         <v>3.6600000000000001E-2</v>
       </c>
-      <c r="L57" s="1" t="s">
+      <c r="J60" s="6"/>
+      <c r="L60" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="M57" t="s">
+      <c r="M60" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    <row r="61" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>62</v>
       </c>
-      <c r="B59" s="2">
-        <v>0.92549999999999999</v>
-      </c>
-      <c r="C59" s="2">
-        <v>0.9829</v>
-      </c>
-      <c r="D59" s="2">
+      <c r="B61" s="2">
+        <v>0.92210000000000003</v>
+      </c>
+      <c r="C61" s="2">
+        <v>0.98150000000000004</v>
+      </c>
+      <c r="D61" s="2">
+        <v>0.99360000000000004</v>
+      </c>
+      <c r="F61" s="2">
+        <v>0.36049999999999999</v>
+      </c>
+      <c r="G61" s="2">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="I61" s="3">
+        <v>3.5799999999999998E-2</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M61" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62" s="2">
+        <v>0.92469999999999997</v>
+      </c>
+      <c r="C62" s="2">
+        <v>0.98270000000000002</v>
+      </c>
+      <c r="D62" s="2">
+        <v>0.99470000000000003</v>
+      </c>
+      <c r="F62" s="2">
+        <v>0.34789999999999999</v>
+      </c>
+      <c r="G62" s="2">
+        <v>8.1100000000000005E-2</v>
+      </c>
+      <c r="I62" s="2">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="L62" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M62" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" s="2">
+        <v>0.92559999999999998</v>
+      </c>
+      <c r="C63" s="2">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="D63" s="2">
         <v>0.99480000000000002</v>
       </c>
-      <c r="F59" s="2">
-        <v>0.34599999999999997</v>
-      </c>
-      <c r="G59" s="2">
+      <c r="F63" s="2">
+        <v>0.34610000000000002</v>
+      </c>
+      <c r="G63" s="2">
         <v>8.1299999999999997E-2</v>
       </c>
-      <c r="I59" s="2">
+      <c r="I63" s="2">
         <v>3.49E-2</v>
       </c>
-      <c r="L59" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>62</v>
-      </c>
-      <c r="B60" s="2">
-        <v>0.92059999999999997</v>
-      </c>
-      <c r="C60" s="2">
-        <v>0.98119999999999996</v>
-      </c>
-      <c r="D60" s="2">
-        <v>0.99390000000000001</v>
-      </c>
-      <c r="F60" s="2">
-        <v>0.37259999999999999</v>
-      </c>
-      <c r="G60" s="2">
-        <v>8.5900000000000004E-2</v>
-      </c>
-      <c r="I60" s="2">
-        <v>3.6600000000000001E-2</v>
-      </c>
-      <c r="L60" s="1" t="s">
-        <v>66</v>
+      <c r="L63" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M63" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>